<commit_message>
gov pov results working
</commit_message>
<xml_diff>
--- a/examples/analysis/dsot/code/input_data/vehicle_config_data_gov.xlsx
+++ b/examples/analysis/dsot/code/input_data/vehicle_config_data_gov.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/kishan_g_pnnl_gov/Documents/Desktop/Gridlabd/DoD/povs/latest_use/july_9_used_data/vehicle_sampling_code_AD_jul9/vehicle_sampling_code_AD/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/kishan_g_pnnl_gov/Documents/Desktop/Gridlabd/DoD/povs/_jul14/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{E9F5E86F-8167-44C3-B587-213A844C2697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88BC0290-6898-4493-8562-77FB33F6F910}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{E9F5E86F-8167-44C3-B587-213A844C2697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B725F36-EE89-4344-822D-F826B2E4DBA3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{605BAD8E-239F-43E3-9343-A726D8892B8A}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="3" xr2:uid="{605BAD8E-239F-43E3-9343-A726D8892B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="MHDV" sheetId="2" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB62E45-33C6-44D6-B81B-0399963B73BB}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +741,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,16 +774,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <f>(24/(569-B2))*100</f>
-        <v>4.2328042328042326</v>
+        <f>(24/(511-B2))*100</f>
+        <v>4.7151277013752457</v>
       </c>
       <c r="D2" s="2">
-        <f>(241/(569-B2))*100</f>
-        <v>42.504409171075835</v>
+        <f>(183/(511-B2))*100</f>
+        <v>35.952848722986246</v>
       </c>
       <c r="E2" s="2">
-        <f>(302/(569-B2))*100</f>
-        <v>53.262786596119923</v>
+        <f>(302/(511-B2))*100</f>
+        <v>59.332023575638502</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -797,16 +797,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f>(32/(685-B3))*100</f>
-        <v>4.6783625730994149</v>
+        <f>(32/(654-B3))*100</f>
+        <v>4.9004594180704446</v>
       </c>
       <c r="D3" s="2">
-        <f>(180/(685-B3))*100</f>
-        <v>26.315789473684209</v>
+        <f>(149/(654-B3))*100</f>
+        <v>22.817764165390507</v>
       </c>
       <c r="E3" s="2">
-        <f>(472/(685-B3))*100</f>
-        <v>69.005847953216374</v>
+        <f>(475/(654-B3))*100</f>
+        <v>72.741194486983147</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -820,16 +820,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <f>(0/(45-B4))*100</f>
+        <f>(0/(41-B4))*100</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>(22/(45-B4))*100</f>
-        <v>51.162790697674424</v>
+        <f>(18/(41-B4))*100</f>
+        <v>46.153846153846153</v>
       </c>
       <c r="E4" s="2">
-        <f>(21/(45-B4))*100</f>
-        <v>48.837209302325576</v>
+        <f>(21/(41-B4))*100</f>
+        <v>53.846153846153847</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85856697-C595-489C-935F-034ABE9C1B9B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,16 +1185,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f>(249/(558-B2))*100</f>
-        <v>44.623655913978496</v>
+        <f>(307/(616-B2))*100</f>
+        <v>49.837662337662337</v>
       </c>
       <c r="D2" s="2">
-        <f>(127/(558-B2))*100</f>
-        <v>22.759856630824373</v>
+        <f>(127/(616-B2))*100</f>
+        <v>20.616883116883116</v>
       </c>
       <c r="E2" s="2">
-        <f>(182/(558-B2))*100</f>
-        <v>32.616487455197138</v>
+        <f>(182/(616-B2))*100</f>
+        <v>29.545454545454547</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,16 +1225,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f>(19/(41-B4))*100</f>
-        <v>46.341463414634148</v>
+        <f>(21/(45-B4))*100</f>
+        <v>46.666666666666664</v>
       </c>
       <c r="D4" s="2">
-        <f>(3/(41-B4))*100</f>
-        <v>7.3170731707317067</v>
+        <f>(5/(45-B4))*100</f>
+        <v>11.111111111111111</v>
       </c>
       <c r="E4" s="2">
-        <f>(19/(41-B4))*100</f>
-        <v>46.341463414634148</v>
+        <f>(19/(45-B4))*100</f>
+        <v>42.222222222222221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>